<commit_message>
Cambios además de pruebas nuevas
En simulación funcionan de forma optima el hecho de guardar cosas en la EEPROM del RTC. Falta saber como comparar además de activar la alarma y posponer en 1 minuto la alarma activa cuando esta se active.
</commit_message>
<xml_diff>
--- a/Reloj_ALarmas.X/Libro2.xlsx
+++ b/Reloj_ALarmas.X/Libro2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hdask\OneDrive\Escritorio\2021-2\MPEI\Proyectos MP LAB\Proyecto 7\Laboratorio_Final_MPEI\Reloj_ALarmas.X\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D23BFEB4-C3AD-4B98-A42C-BBA28F528E51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{449076AF-D98A-4802-A10E-B4C6113D9ECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{9891FC35-E95C-4A67-AEA0-7E9103FFB327}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="31">
   <si>
     <t>M</t>
   </si>
@@ -117,16 +117,16 @@
     <t>Pantalla default</t>
   </si>
   <si>
-    <t>HA</t>
-  </si>
-  <si>
-    <t>HB</t>
-  </si>
-  <si>
-    <t>MA</t>
-  </si>
-  <si>
-    <t>MB</t>
+    <t>f</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>p</t>
   </si>
 </sst>
 </file>
@@ -481,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4C7A4D8-A878-447F-B829-E22F26091E35}">
-  <dimension ref="A2:T19"/>
+  <dimension ref="A2:T27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -943,46 +943,176 @@
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" t="s">
+        <v>5</v>
+      </c>
+      <c r="F20" t="s">
+        <v>2</v>
+      </c>
+      <c r="G20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" t="s">
         <v>9</v>
       </c>
-      <c r="C19" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" t="s">
-        <v>2</v>
-      </c>
-      <c r="E19" t="s">
-        <v>13</v>
-      </c>
-      <c r="F19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G19" t="s">
+      <c r="E22" t="s">
         <v>23</v>
       </c>
-      <c r="H19" t="s">
-        <v>5</v>
-      </c>
-      <c r="I19" t="s">
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" t="s">
+        <v>19</v>
+      </c>
+      <c r="D26" t="s">
         <v>21</v>
       </c>
-      <c r="K19" t="s">
-        <v>27</v>
-      </c>
-      <c r="L19" t="s">
-        <v>28</v>
-      </c>
-      <c r="M19" t="s">
-        <v>11</v>
-      </c>
-      <c r="N19" t="s">
-        <v>29</v>
-      </c>
-      <c r="O19" t="s">
+      <c r="E26" t="s">
+        <v>22</v>
+      </c>
+      <c r="F26" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" t="s">
         <v>30</v>
+      </c>
+      <c r="D27" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" t="s">
+        <v>5</v>
+      </c>
+      <c r="G27" t="s">
+        <v>20</v>
+      </c>
+      <c r="H27" t="s">
+        <v>6</v>
+      </c>
+      <c r="I27" t="s">
+        <v>2</v>
+      </c>
+      <c r="J27" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>